<commit_message>
test cases for bmw and att
</commit_message>
<xml_diff>
--- a/bmw/src/test/resources/BMWTestData.xlsx
+++ b/bmw/src/test/resources/BMWTestData.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erdosa\IdeaProjects\Team2_BDDFramework\bmw\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0EF7E3D-22EC-443E-8B0E-9AC640EABA0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197E66CD-54B2-44B2-80D8-0A3A2BC0738B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3997E247-4C2D-43A7-BB22-35D882DF67F9}"/>
+    <workbookView xWindow="5115" yWindow="720" windowWidth="15375" windowHeight="7005" activeTab="2" xr2:uid="{3997E247-4C2D-43A7-BB22-35D882DF67F9}"/>
   </bookViews>
   <sheets>
     <sheet name="HelpBoxText" sheetId="1" r:id="rId1"/>
+    <sheet name="Answers" sheetId="2" r:id="rId2"/>
+    <sheet name="QuestionsTitles" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>All transactions related to the optional BMW Ultimate Protection Program are governed solely by the provisions of each agreement. This website provides general information about the BMW Ultimate Protection Program Products and should not be solely relied upon when purchasing coverage. Please refer to the BMW Ultimate Protection Program Multi-Coverage Service Contract for details of terms, conditions, and specific coverage details, including limitations and exclusions. Coverage may vary by state. The obligor/administrator of the Tire &amp; Wheel Protection, Paintless Dent Repair and Windshield Protection coverages included in the BMW Protection Package is Safe-Guard Products International, LLC., except in Florida where the obligor/administrator of the Tire &amp; Wheel Protection and Paintless Dent Repair coverages is Safe-Guard Warranty Corporation, Florida License # 60126, Two Concourse Parkway, Suite 500, Atlanta, GA 30328, 1-800-269-4559. The obligor/administrator of the BMW Key Protection coverage is SafeRide Motor Club, Inc., 4287 Beltline Road, #238, Addison, TX 75001, 1-844-287-4036. The administrator of BMW Guaranteed Auto Protection and BMW Lease Protection is Safe-Guard Products International, LLC., Two Concourse Parkway, Suite 500, Atlanta, GA, 30328, 1-800-269-4559, except in Indiana where the administrator of BMW Guaranteed Auto Protection is Safe-Guard Warranty Corporation.</t>
   </si>
@@ -34,6 +36,71 @@
   </si>
   <si>
     <t>Offer subject to credit approval through BMW Financial Services and verification of graduation and employment. Recent graduate means graduation from an accredited college or university with a doctorate, graduate, undergraduate, or associate's degree earned within the previous 24 months, or is eligible to graduate within the next 6 months and has a verifiable offer of employment. To qualify, you must have a minimum of 6 months of credit on file and no previous derogatory credit on any credit lines. Finance and lease terms based on credit score. See your BMW Client Advisor for most current program.</t>
+  </si>
+  <si>
+    <t>BMW Financial Services offers a variety of easy, convenient payment methods.
+Online with your My BMW account
+Easily manage your account online with My BMW. From here, you can make one-time electronic payments, enroll in EasyPay automatic payments, sign up for Paperless Statements, view your Account Statements, and more.
+Log in or create your account today at mybmw.bmwusa.com
+Pay By Phone
+Call 800-578-5000 and make a one-time payment with your checking/savings account or debit card for the same day, or schedule your payment for a future date.
+Pay By Mail
+Tear off and return the bottom portion of your Account Statement with your payment. (If you're signed up for paperless statements, print the return portion). Make checks payable to BMW Financial Services and include your 10-digit BMW Financial Services account number.</t>
+  </si>
+  <si>
+    <t>Account Statements are delivered approximately 14 days before a payment is due. You'll receive a notification by mail, or by email if you're enrolled in paperless statements.
+You can also view your Account Statement any time by signing in to My BMW.</t>
+  </si>
+  <si>
+    <t>Payments are first credited to unpaid finance charges, then to the outstanding principal balance, then to any outstanding fees. Your Account Statement will break down how your payments have been allocated.
+Amortization schedules are always available through your My BMW account.</t>
+  </si>
+  <si>
+    <t>While debit cards are acceptable, we unfortunately cannot accept credit cards for regular monthly payments.</t>
+  </si>
+  <si>
+    <t>Grace periods – the amount of time between a due date and the assessment of late fees – are regulated by state governments. Please refer to the Account Summary section of your Account Statement to determine if you are eligible for a grace period.</t>
+  </si>
+  <si>
+    <t>Yes. If you pay more than the Total Amount Due, the extra payment will be applied to your principal balance. This may reduce the interest you pay over the life of your account and may reduce your final payment or shorten the term of your financing agreement.</t>
+  </si>
+  <si>
+    <t>Payment credits are applied on your scheduled due date and will be reflected on your Account Statement.</t>
+  </si>
+  <si>
+    <t>Late payments (more than 29 days past due), missed payments, or other defaults on your account may be reflected on your credit report. In accordance with Federal law, you are hereby notified that a negative credit report reflecting on your credit records may be submitted to a credit reporting agency if you fail to fulfill the terms of your credit obligation.</t>
+  </si>
+  <si>
+    <t>1
+What payment options are available?</t>
+  </si>
+  <si>
+    <t>2
+When will I receive my monthly Account Statements?</t>
+  </si>
+  <si>
+    <t>3
+How are my payments applied?</t>
+  </si>
+  <si>
+    <t>4
+Can I make a payment with my debit or credit card?</t>
+  </si>
+  <si>
+    <t>5
+Is there a grace period for late charges?</t>
+  </si>
+  <si>
+    <t>6
+Can I make a payment greater than my regular scheduled monthly payment?</t>
+  </si>
+  <si>
+    <t>7
+How are payment credits applied?</t>
+  </si>
+  <si>
+    <t>8
+What happens if I miss a payment?</t>
   </si>
 </sst>
 </file>
@@ -69,8 +136,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,7 +457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5C4662-FB75-4F4C-938A-1E78AD0C825B}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -414,4 +484,118 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D2CA0A-929D-447C-8AF1-C0DA54454337}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="125.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E1F1B2-53A7-44BC-8514-1D4896355A3C}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection sqref="A1:A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>